<commit_message>
Update the dates objects
</commit_message>
<xml_diff>
--- a/dates_formats.xlsx
+++ b/dates_formats.xlsx
@@ -149,9 +149,9 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="3">
-    <numFmt numFmtId="166" formatCode="yyyy/m/d;@"/>
-    <numFmt numFmtId="168" formatCode="[$-1009]mmmm\ d\,\ yyyy;@"/>
-    <numFmt numFmtId="170" formatCode="[$-1C09]dd\ mmmm\ yyyy;@"/>
+    <numFmt numFmtId="164" formatCode="yyyy/m/d;@"/>
+    <numFmt numFmtId="165" formatCode="[$-1009]mmmm\ d\,\ yyyy;@"/>
+    <numFmt numFmtId="166" formatCode="[$-1C09]dd\ mmmm\ yyyy;@"/>
   </numFmts>
   <fonts count="18" x14ac:knownFonts="1">
     <font>
@@ -630,12 +630,13 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="17" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="168" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="170" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -960,7 +961,7 @@
   <dimension ref="A1:G23"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E2" sqref="E2:E23"/>
+      <selection activeCell="G2" sqref="G2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1013,7 +1014,7 @@
       <c r="F2" t="s">
         <v>8</v>
       </c>
-      <c r="G2" s="1">
+      <c r="G2" s="5">
         <v>42755</v>
       </c>
     </row>

</xml_diff>